<commit_message>
Update Excel - Row-Column values (for a given cell).xlsx
</commit_message>
<xml_diff>
--- a/excel/Excel - Row-Column values (for a given cell).xlsx
+++ b/excel/Excel - Row-Column values (for a given cell).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\Coding\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B861161E-4D05-4076-939C-C177450EEFDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E72B8C2-10CC-4E3F-A6D7-A7F7F3A8AFDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3FF85B8A-3267-462A-9BA5-5DC5D40E610F}"/>
   </bookViews>
@@ -380,7 +380,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="A19" sqref="A19:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>